<commit_message>
Load table for mrp calculation results
</commit_message>
<xml_diff>
--- a/R-dataprocessor/submodules/02_MRP_Drug_Disease/R-MRP_Drug_Disease/inst/extdata/mrp_drug_disease.xlsx
+++ b/R-dataprocessor/submodules/02_MRP_Drug_Disease/R-MRP_Drug_Disease/inst/extdata/mrp_drug_disease.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="mrp_drug_disease" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -418,7 +418,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>